<commit_message>
Get all 6 major scenarios built in to habitat attributes workbook
</commit_message>
<xml_diff>
--- a/srt_figures/hab_attributes_template.xlsx
+++ b/srt_figures/hab_attributes_template.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/calebfogel/Documents/Work_NOAA/ASRP/asrp/srt_figures/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756E292F-BAA0-8A4E-95F8-073B685F9321}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="GSU habitat attributes" sheetId="1" r:id="rId1"/>
+    <sheet name="Subbasin habitat attributes" sheetId="6" r:id="rId2"/>
+    <sheet name="EDR habitat attributes" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="27">
   <si>
     <t>GSU</t>
   </si>
@@ -39,38 +45,82 @@
     <t>Average temperature (Historical, °C)</t>
   </si>
   <si>
-    <t>Floodplain area (current, ha)</t>
-  </si>
-  <si>
-    <t>Floodplain area (historical, ha)</t>
-  </si>
-  <si>
-    <t>Floodplain restoration potential (area, ha)</t>
+    <t>Spawning area (low wood, m^2)</t>
+  </si>
+  <si>
+    <t>Spawning area (high wood, m^2)</t>
+  </si>
+  <si>
+    <t>Percent passage (current)</t>
+  </si>
+  <si>
+    <t>Percent passage (historical)</t>
+  </si>
+  <si>
+    <t>Restoration potential (percent passage)</t>
+  </si>
+  <si>
+    <t>Beaver intrinsic potential</t>
+  </si>
+  <si>
+    <t>Rank (beaver intrinsic potential)</t>
+  </si>
+  <si>
+    <t>Rank (passage restoration potential)</t>
+  </si>
+  <si>
+    <t>Floodplain area (current)</t>
+  </si>
+  <si>
+    <t>Floodplain area (historical)</t>
+  </si>
+  <si>
+    <t>Floodplain restoration potential (area, Ha)</t>
+  </si>
+  <si>
+    <t>Rank (floodplain restoration potential)</t>
   </si>
   <si>
     <t>Shade restoration potential (average temperature, °C)</t>
   </si>
   <si>
-    <t>Spawning area (low wood, m^2)</t>
-  </si>
-  <si>
-    <t>Spawning area (high wood, m^2)</t>
-  </si>
-  <si>
-    <t>Spawning gravel restoration potential (area, m^2)</t>
+    <t>Rank (shade restoration potential)</t>
+  </si>
+  <si>
+    <t>Spawning gravel restoration potential ( area, m^2)</t>
+  </si>
+  <si>
+    <t>Rank (spawning gravel restoration potential)</t>
+  </si>
+  <si>
+    <t>Percent fine sediment (current)</t>
+  </si>
+  <si>
+    <t>Percent fine sediment (historical)</t>
+  </si>
+  <si>
+    <t>Restoration potential (percent fine sediment</t>
+  </si>
+  <si>
+    <t>Rank (fine sediment restoraion potential)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -114,9 +164,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -128,6 +181,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -176,7 +232,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -209,9 +265,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -244,6 +317,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -419,63 +509,91 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:X1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="37" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
+    <col min="2" max="43" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
+      <c r="S1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -485,25 +603,200 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7226F900-C744-AC46-94D9-15693DCB75BC}">
+  <dimension ref="A1:AA1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:AA1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="4" width="30.6640625" customWidth="1"/>
+    <col min="5" max="41" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FA31869-8224-C64D-B4F1-A510F5FBF87D}">
+  <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:X1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
+    <col min="2" max="38" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add colors to hab attributes template
</commit_message>
<xml_diff>
--- a/srt_figures/hab_attributes_template.xlsx
+++ b/srt_figures/hab_attributes_template.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10510"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/calebfogel/Documents/Work_NOAA/ASRP/asrp/srt_figures/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756E292F-BAA0-8A4E-95F8-073B685F9321}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16440" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GSU habitat attributes" sheetId="1" r:id="rId1"/>
@@ -27,9 +21,6 @@
     <t>GSU</t>
   </si>
   <si>
-    <t>Subbasin number</t>
-  </si>
-  <si>
     <t>Subbasin</t>
   </si>
   <si>
@@ -103,12 +94,15 @@
   </si>
   <si>
     <t>Rank (fine sediment restoraion potential)</t>
+  </si>
+  <si>
+    <t>Subbasin_num</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -123,7 +117,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,6 +127,42 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD898CA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -164,12 +194,75 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -181,9 +274,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -232,7 +322,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -265,26 +355,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -317,23 +390,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -509,91 +565,91 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:X1"/>
+      <selection sqref="A1:X1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" customWidth="1"/>
-    <col min="2" max="43" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="43" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:24" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="S1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="15" t="s">
         <v>25</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -603,102 +659,102 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7226F900-C744-AC46-94D9-15693DCB75BC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:AA1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="4" width="30.6640625" customWidth="1"/>
-    <col min="5" max="41" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="41" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:27" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="U1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="8" t="s">
         <v>25</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -708,91 +764,91 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FA31869-8224-C64D-B4F1-A510F5FBF87D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:X1"/>
+      <selection sqref="A1:X1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" customWidth="1"/>
-    <col min="2" max="38" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="38" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:24" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="S1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="22" t="s">
         <v>25</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>